<commit_message>
Results TAR and M-TAR (Enders & Granger, 1998)
</commit_message>
<xml_diff>
--- a/Proyecto Interno/working-papers/working-paper-aecm/output/ts-ecm/261225_table2_longrun.xlsx
+++ b/Proyecto Interno/working-papers/working-paper-aecm/output/ts-ecm/261225_table2_longrun.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,490 +360,280 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>pair</t>
+          <t>city</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Cali - b</t>
+          <t>articulo_ipc</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Cali - se</t>
+          <t>b</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Cali - p-value</t>
+          <t>se</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Bogotá - b</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Bogotá - se</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Bogotá - p-value</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Medellín - b</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Medellín - se</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Medellín - p-value</t>
+          <t>p-value</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ARROZ PARA SECO / Arroz de primera</t>
-        </is>
-      </c>
-      <c r="B2">
-        <v>0.8672185974609786</v>
+          <t>Bogotá</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ARROZ PARA SECO</t>
+        </is>
       </c>
       <c r="C2">
-        <v>0.04189595233140812</v>
+        <v>0.8597755805941806</v>
       </c>
       <c r="D2">
-        <v>2.828357343525357E-29</v>
+        <v>0.06146939335618964</v>
       </c>
       <c r="E2">
-        <v>0.8597755805941806</v>
-      </c>
-      <c r="F2">
-        <v>0.06146939335618964</v>
-      </c>
-      <c r="G2">
         <v>1.077942175711338E-20</v>
-      </c>
-      <c r="H2">
-        <v>1.005309314498095</v>
-      </c>
-      <c r="I2">
-        <v>0.06891808130255779</v>
-      </c>
-      <c r="J2">
-        <v>1.486037087339282E-21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CEBOLLA CABEZONA / Cebolla cabezona blanca</t>
-        </is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ARROZ PARA SECO</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>0.8672185974609786</v>
+      </c>
+      <c r="D3">
+        <v>0.04189595233140812</v>
       </c>
       <c r="E3">
-        <v>0.5642186112401515</v>
-      </c>
-      <c r="F3">
-        <v>0.1179340911541281</v>
-      </c>
-      <c r="G3">
-        <v>1.128221550541083E-05</v>
-      </c>
-      <c r="H3">
-        <v>0.7303457209125235</v>
-      </c>
-      <c r="I3">
-        <v>0.124233838170302</v>
-      </c>
-      <c r="J3">
-        <v>1.866415714325836E-07</v>
+        <v>2.828357343525357E-29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CEBOLLA CABEZONA / Cebolla cabezona blanca bogotana</t>
-        </is>
-      </c>
-      <c r="B4">
-        <v>0.6966571940722384</v>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ARROZ PARA SECO</t>
+        </is>
       </c>
       <c r="C4">
-        <v>0.1002874973044226</v>
+        <v>1.005309314498095</v>
       </c>
       <c r="D4">
-        <v>2.862097712128018E-09</v>
+        <v>0.06891808130255779</v>
+      </c>
+      <c r="E4">
+        <v>1.486037087339282E-21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PAPA / Papa R-12 negra</t>
-        </is>
+          <t>Bogotá</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>PAPA</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>0.5335352352416299</v>
+      </c>
+      <c r="D5">
+        <v>0.1115555640748547</v>
       </c>
       <c r="E5">
-        <v>0.5335352352416299</v>
-      </c>
-      <c r="F5">
-        <v>0.1115555640748547</v>
-      </c>
-      <c r="G5">
         <v>1.134356642927936E-05</v>
-      </c>
-      <c r="H5">
-        <v>0.882887112426149</v>
-      </c>
-      <c r="I5">
-        <v>0.1218388986050033</v>
-      </c>
-      <c r="J5">
-        <v>8.735394106006289E-10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PAPA / Papa capira</t>
-        </is>
-      </c>
-      <c r="B6">
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PAPA</t>
+        </is>
+      </c>
+      <c r="C6">
         <v>0.7583601640417631</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.1221080690603679</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>5.159561390843883E-08</v>
-      </c>
-      <c r="H6">
-        <v>1.022196701484384</v>
-      </c>
-      <c r="I6">
-        <v>0.1231100642796551</v>
-      </c>
-      <c r="J6">
-        <v>1.325729852449282E-11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PAPA / Papa nevada</t>
-        </is>
-      </c>
-      <c r="H7">
-        <v>0.7540131927712588</v>
-      </c>
-      <c r="I7">
-        <v>0.08297037165342941</v>
-      </c>
-      <c r="J7">
-        <v>6.069995105361257E-13</v>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>PAPA</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>1.022196701484384</v>
+      </c>
+      <c r="D7">
+        <v>0.1231100642796551</v>
+      </c>
+      <c r="E7">
+        <v>1.325729852449282E-11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PAPA / Papa parda pastusa</t>
-        </is>
-      </c>
-      <c r="B8">
-        <v>0.7000827741948205</v>
+          <t>Bogotá</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PLÁTANO</t>
+        </is>
       </c>
       <c r="C8">
-        <v>0.1075556950875227</v>
+        <v>0.7423630237190562</v>
       </c>
       <c r="D8">
-        <v>1.605463030963244E-08</v>
+        <v>0.08430686378385766</v>
       </c>
       <c r="E8">
-        <v>0.5838931240877929</v>
-      </c>
-      <c r="F8">
-        <v>0.1310416871134433</v>
-      </c>
-      <c r="G8">
-        <v>3.63885256205301E-05</v>
+        <v>1.832721421380436E-12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>PAPA / Papa suprema</t>
-        </is>
-      </c>
-      <c r="B9">
-        <v>0.658723978395932</v>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PLÁTANO</t>
+        </is>
       </c>
       <c r="C9">
-        <v>0.1165971846902779</v>
+        <v>0.7291642526870556</v>
       </c>
       <c r="D9">
-        <v>4.495403710456148E-07</v>
+        <v>0.06306868110295819</v>
       </c>
       <c r="E9">
-        <v>0.4746251339074692</v>
-      </c>
-      <c r="F9">
-        <v>0.1117089221507378</v>
-      </c>
-      <c r="G9">
-        <v>7.47407341856761E-05</v>
+        <v>5.190396827295085E-17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PAPA / Papa única</t>
-        </is>
-      </c>
-      <c r="B10">
-        <v>0.5102966925084667</v>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>PLÁTANO</t>
+        </is>
       </c>
       <c r="C10">
-        <v>0.09770711875021475</v>
+        <v>0.7585013546119171</v>
       </c>
       <c r="D10">
-        <v>2.251588060286905E-06</v>
+        <v>0.09791222800752789</v>
       </c>
       <c r="E10">
-        <v>0.4133789283112398</v>
-      </c>
-      <c r="F10">
-        <v>0.1018323154925061</v>
-      </c>
-      <c r="G10">
-        <v>0.0001423896219966501</v>
+        <v>1.200378689278605E-10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PLÁTANO / Plátano guineo</t>
-        </is>
+          <t>Bogotá</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>YUCA</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>0.4280256455811501</v>
+      </c>
+      <c r="D11">
+        <v>0.04902700477690952</v>
       </c>
       <c r="E11">
-        <v>0.7712365963980458</v>
-      </c>
-      <c r="F11">
-        <v>0.1184833629597216</v>
-      </c>
-      <c r="G11">
-        <v>1.604115100338973E-08</v>
-      </c>
-      <c r="H11">
-        <v>0.6262721091371228</v>
-      </c>
-      <c r="I11">
-        <v>0.1000602160557386</v>
-      </c>
-      <c r="J11">
-        <v>4.272499347667159E-08</v>
+        <v>2.461174605519535E-12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PLÁTANO / Plátano hartón maduro</t>
-        </is>
-      </c>
-      <c r="H12">
-        <v>0.7298009116969256</v>
-      </c>
-      <c r="I12">
-        <v>0.1047210860396661</v>
-      </c>
-      <c r="J12">
-        <v>2.619541397726329E-09</v>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>YUCA</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>0.5810042832793612</v>
+      </c>
+      <c r="D12">
+        <v>0.05030803954711753</v>
+      </c>
+      <c r="E12">
+        <v>5.432594097677105E-17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PLÁTANO / Plátano hartón verde</t>
-        </is>
-      </c>
-      <c r="B13">
-        <v>0.7291642526870556</v>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>YUCA</t>
+        </is>
       </c>
       <c r="C13">
-        <v>0.06306868110295819</v>
+        <v>0.5375944788025322</v>
       </c>
       <c r="D13">
-        <v>5.190396827295085E-17</v>
-      </c>
-      <c r="H13">
-        <v>0.7585013546119171</v>
-      </c>
-      <c r="I13">
-        <v>0.09791222800752789</v>
-      </c>
-      <c r="J13">
-        <v>1.200378689278605E-10</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>PLÁTANO / Plátano hartón verde llanero</t>
-        </is>
-      </c>
-      <c r="E14">
-        <v>0.7566951174791167</v>
-      </c>
-      <c r="F14">
-        <v>0.07536183147056857</v>
-      </c>
-      <c r="G14">
-        <v>1.525406681337241E-14</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>TOMATE / Tomate chonto</t>
-        </is>
-      </c>
-      <c r="E15">
-        <v>0.518741753955081</v>
-      </c>
-      <c r="F15">
-        <v>0.1199997275846435</v>
-      </c>
-      <c r="G15">
-        <v>5.786810624791092E-05</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>TOMATE / Tomate larga vida</t>
-        </is>
-      </c>
-      <c r="B16">
-        <v>0.8729995475250916</v>
-      </c>
-      <c r="C16">
-        <v>0.1730810943596067</v>
-      </c>
-      <c r="D16">
-        <v>4.370346081427119E-06</v>
-      </c>
-      <c r="E16">
-        <v>0.4038658847368593</v>
-      </c>
-      <c r="F16">
-        <v>0.08029370851800757</v>
-      </c>
-      <c r="G16">
-        <v>4.602023089008143E-06</v>
-      </c>
-      <c r="H16">
-        <v>0.6486137790749836</v>
-      </c>
-      <c r="I16">
-        <v>0.1169001865809834</v>
-      </c>
-      <c r="J16">
-        <v>6.606244706686408E-07</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>YUCA / Yuca ICA</t>
-        </is>
-      </c>
-      <c r="B17">
-        <v>0.5810042832793612</v>
-      </c>
-      <c r="C17">
-        <v>0.05030803954711753</v>
-      </c>
-      <c r="D17">
-        <v>5.432594097677105E-17</v>
-      </c>
-      <c r="H17">
-        <v>0.5375944788025322</v>
-      </c>
-      <c r="I17">
         <v>0.04468819798692237</v>
       </c>
-      <c r="J17">
+      <c r="E13">
         <v>9.522160735313239E-18</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>YUCA / Yuca llanera</t>
-        </is>
-      </c>
-      <c r="E18">
-        <v>0.4280256455811501</v>
-      </c>
-      <c r="F18">
-        <v>0.04902700477690952</v>
-      </c>
-      <c r="G18">
-        <v>2.461174605519535E-12</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>ZANAHORIA / Zanahoria</t>
-        </is>
-      </c>
-      <c r="E19">
-        <v>0.4895066012246989</v>
-      </c>
-      <c r="F19">
-        <v>0.1246280354492657</v>
-      </c>
-      <c r="G19">
-        <v>0.0002210451286250006</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>ZANAHORIA / Zanahoria bogotana</t>
-        </is>
-      </c>
-      <c r="B20">
-        <v>0.5500143459863069</v>
-      </c>
-      <c r="C20">
-        <v>0.1349833297373089</v>
-      </c>
-      <c r="D20">
-        <v>0.0001352451441017405</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>ZANAHORIA / Zanahoria larga vida</t>
-        </is>
-      </c>
-      <c r="H21">
-        <v>0.6389480613455027</v>
-      </c>
-      <c r="I21">
-        <v>0.1217318950835173</v>
-      </c>
-      <c r="J21">
-        <v>2.042615594147354E-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>